<commit_message>
Update file_handler.py for converter export with different column size.
</commit_message>
<xml_diff>
--- a/test/test_output/test_equalize.xlsx
+++ b/test/test_output/test_equalize.xlsx
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>CL(1'-[18:1(9Z)/18:2(9Z,12Z)],3'-[18:2(9Z,12Z)/18:2(9Z,12Z)])</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2623,11 +2623,7 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">

</xml_diff>